<commit_message>
summer sucker model updates
</commit_message>
<xml_diff>
--- a/data/life_history_model.xlsx
+++ b/data/life_history_model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cas39\github\sucker_phenotypes\raw-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cas39\github\suckerIPM\suckerIPM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19400" windowHeight="10730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19400" windowHeight="10730"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="82">
   <si>
     <t>water</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>average allele frequency polarized by White Sucker reference genome</t>
+  </si>
+  <si>
+    <t>genotype_cands</t>
   </si>
 </sst>
 </file>
@@ -1074,15 +1077,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="12" max="12" width="13.81640625" customWidth="1"/>
+    <col min="16" max="17" width="13.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1122,8 +1129,11 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1161,7 +1171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1199,7 +1209,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1240,7 +1250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1316,7 +1326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1392,7 +1402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1430,7 +1440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1468,7 +1478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1506,7 +1516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1544,7 +1554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1581,8 +1591,11 @@
       <c r="M13">
         <v>0.865222728</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N13">
+        <v>0.49671368965517199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1619,8 +1632,11 @@
       <c r="M14">
         <v>0.87158818699999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N14">
+        <v>0.52776496078431301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1657,8 +1673,11 @@
       <c r="M15">
         <v>0.90272045300000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N15">
+        <v>0.54641756140350795</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1698,8 +1717,11 @@
       <c r="M16">
         <v>0.90852398899999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N16">
+        <v>0.49549013461538399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1736,8 +1758,11 @@
       <c r="M17">
         <v>0.88404070700000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N17">
+        <v>0.59143376363636302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1774,8 +1799,11 @@
       <c r="M18">
         <v>0.91964525399999997</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N18">
+        <v>0.58041996226415005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1815,8 +1843,11 @@
       <c r="M19">
         <v>0.95314133400000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N19">
+        <v>0.47648431578947298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1856,8 +1887,11 @@
       <c r="M20">
         <v>0.89180337499999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N20">
+        <v>0.548971372881355</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1897,8 +1931,11 @@
       <c r="M21">
         <v>0.87850314200000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N21">
+        <v>0.70167063461538404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1938,8 +1975,11 @@
       <c r="M22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1979,8 +2019,11 @@
       <c r="M23">
         <v>0.90066339900000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N23">
+        <v>0.63123343999999904</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2020,8 +2063,11 @@
       <c r="M24">
         <v>0.83172289200000005</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N24">
+        <v>0.59898692857142799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2058,8 +2104,11 @@
       <c r="M25">
         <v>1.543516903</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N25">
+        <v>0.33357199999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2096,8 +2145,11 @@
       <c r="M26">
         <v>1.5501386029999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N26">
+        <v>1.48983146153846</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2137,8 +2189,11 @@
       <c r="M27">
         <v>0.87440395000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N27">
+        <v>0.57030908474576203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2175,8 +2230,11 @@
       <c r="M28">
         <v>1.2887658989999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N28">
+        <v>0.64000906666666602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -2216,8 +2274,11 @@
       <c r="M29">
         <v>1.287705651</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N29">
+        <v>0.89439324242424201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2254,8 +2315,11 @@
       <c r="M30">
         <v>1.5340655489999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N30">
+        <v>1.0080063090908999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2295,8 +2359,11 @@
       <c r="M31">
         <v>1.193954441</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N31">
+        <v>0.647034446428571</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -2336,8 +2403,11 @@
       <c r="M32">
         <v>1.14395117</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N32">
+        <v>0.62470725999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -2374,8 +2444,11 @@
       <c r="M33">
         <v>1.2970586740000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N33">
+        <v>1.46621285185185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -2412,8 +2485,11 @@
       <c r="M34">
         <v>1.583188547</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N34">
+        <v>1.51342416949152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2453,8 +2529,11 @@
       <c r="M35" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -2494,8 +2573,11 @@
       <c r="M36">
         <v>1.7639901360000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N36">
+        <v>1.7218141052631499</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -2535,8 +2617,11 @@
       <c r="M37">
         <v>0.82543162199999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N37">
+        <v>1.4978734909090901</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -2573,8 +2658,11 @@
       <c r="M38">
         <v>1.517255936</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N38">
+        <v>1.0374610612244799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2614,8 +2702,11 @@
       <c r="M39">
         <v>1.522245531</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N39">
+        <v>1.42163229411764</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2655,8 +2746,11 @@
       <c r="M40">
         <v>0.91255043700000005</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N40">
+        <v>0.97233009999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -2696,8 +2790,11 @@
       <c r="M41">
         <v>0.99307402600000005</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N41">
+        <v>0.87030355172413698</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2737,8 +2834,11 @@
       <c r="M42">
         <v>1.1443957119999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N42">
+        <v>0.49717301818181803</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2778,8 +2878,11 @@
       <c r="M43">
         <v>0.97758020700000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N43">
+        <v>0.73118903636363597</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -2816,8 +2919,11 @@
       <c r="M44">
         <v>1.001621198</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -2854,8 +2960,11 @@
       <c r="M45">
         <v>0.90821986700000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N45">
+        <v>0.58192392857142805</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2892,8 +3001,11 @@
       <c r="M46">
         <v>1.2348675410000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N46">
+        <v>1.3243682068965501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2930,8 +3042,11 @@
       <c r="M47">
         <v>1.3351946589999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N47">
+        <v>0.53721688679245205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2967,6 +3082,9 @@
       </c>
       <c r="M48">
         <v>1.2105930659999999</v>
+      </c>
+      <c r="N48">
+        <v>0.86304875000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2978,7 +3096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>